<commit_message>
Revert "added a special group - 'New Signs' in home page, categories page"
</commit_message>
<xml_diff>
--- a/public/assets/BIM.xlsx
+++ b/public/assets/BIM.xlsx
@@ -7,91 +7,91 @@
     <sheet state="visible" name="Group" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_49E7F3CE_F40C_4FED_BEF8_26F090EE4EAB_.wvu.FilterData">BIM!$A$562:$L$572</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_724DC91F_FF1E_468C_B992_B1D0F51CCC52_.wvu.FilterData">BIM!$A$1:$O$1125</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_8232B643_36E7_487B_B1D6_FD3DA06BF1E9_.wvu.FilterData">BIM!$A$775:$L$811</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_8BD75489_4874_47F0_8DF3_393379AB259B_.wvu.FilterData">BIM!$A$891:$L$1023</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_A856CC1B_B362_4556_ACE2_C976256EBF5B_.wvu.FilterData">BIM!$A$573:$L$584</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_DBDF39FA_7899_4557_B3BC_352C416503A3_.wvu.FilterData">BIM!$A$994:$L$1005</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_9E47DD61_E6DE_488B_80BA_967A50C8AB36_.wvu.FilterData">BIM!$A$565:$L$574</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_BE442BB6_3A31_442F_B924_D13D0F598ECC_.wvu.FilterData">BIM!$A$875:$L$890</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_DE900718_0161_4792_8EAB_C58F78F69250_.wvu.FilterData">BIM!$A$1009:$L$1031</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_030204D7_095F_4354_969B_56C1AA7143AE_.wvu.FilterData">BIM!$A$1039:$L$1074</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_D8E7AD2B_1D6A_4A53_BADF_5738E01F788C_.wvu.FilterData">BIM!$A$267:$L$314</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_7B44AC12_E6B4_4313_993B_10F7132B892F_.wvu.FilterData">BIM!$A$315:$L$334</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_AF68C2CF_34E8_443E_B4ED_BB66CB150D6B_.wvu.FilterData">BIM!$A$37:$L$69</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_CA698D16_9134_4DB4_984A_29693DB788A8_.wvu.FilterData">BIM!$A$1:$N$1125</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_743AD89C_320C_4C4C_BC5F_7EC0A02EECDE_.wvu.FilterData">BIM!$A$521:$L$531</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_A7B4F8D0_C2B2_4D23_888B_901C02EDA207_.wvu.FilterData">BIM!$A$533:$L$565</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_43C9EAE1_EEE7_465A_B2FE_FCC5D6144576_.wvu.FilterData">BIM!$A$718:$L$769</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_D6318188_C0E0_4364_A149_FD9E8D671A1B_.wvu.FilterData">BIM!$A$770:$L$793</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_2039A978_ADAF_4711_8B07_046A7AD53BA6_.wvu.FilterData">BIM!$A$625:$L$658</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_C6F25ED8_01F5_4EC6_BA59_11F1B290E9F7_.wvu.FilterData">BIM!$A$923:$L$960</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_3D296FF4_2091_4F77_BB20_5342594B263E_.wvu.FilterData">BIM!$A$2:$L$36</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_560CED10_97E3_4B8F_9E2D_42501DEDD37A_.wvu.FilterData">BIM!$A$267:$H$314</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_FAE9710F_D2BA_4EBD_88A7_23B01C8DBCFC_.wvu.FilterData">BIM!$A$710:$L$724</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_C330DD12_F7AD_4A16_8E93_F60E7DD26815_.wvu.FilterData">BIM!$A$144:$L$266</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_EF393267_77E9_4937_B374_A059A55A3DDA_.wvu.FilterData">BIM!$A$1:$O$1125</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_3A76F548_2F88_4245_B104_5C766A91C956_.wvu.FilterData">BIM!$A$803:$L$874</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_9DF68346_E0CA_4FA3_B5D1_1AD86B191463_.wvu.FilterData">BIM!$A$573:$L$591</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_1A8878F0_0412_4D55_9C2F_095CAD9E6CFA_.wvu.FilterData">BIM!$A$970:$L$993</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_0ECEE141_0B77_44E5_A6DE_68B5A15450B4_.wvu.FilterData">BIM!$A$429:$L$462</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_AABB1EE6_8061_4BBE_83FC_087E9C58414A_.wvu.FilterData">BIM!$A$335:$L$346</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_EBA9F249_1672_448E_8531_16FD1942FCAD_.wvu.FilterData">BIM!$A$832:$L$863</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_B7D1E82B_A5E5_4C14_9C86_B61A78ED8084_.wvu.FilterData">BIM!$A$728:$L$774</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_48CE27A7_5499_4811_A41E_787093C14E7E_.wvu.FilterData">BIM!$A$794:$L$802</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_E460850B_B72B_48C4_B246_11D0D04F03F5_.wvu.FilterData">BIM!$A$1:$O$1125</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_92BEF0B2_FF4A_4089_8EE6_8E4DADA938AF_.wvu.FilterData">BIM!$A$75:$L$157</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_9E4183D2_CC5A_4D20_BB9A_2F013C0CE815_.wvu.FilterData">BIM!$A$77:$L$128</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_0909C5DC_ED19_4D4A_9DB0_5392CF96C4D4_.wvu.FilterData">BIM!$A$551:$L$565</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_F436789B_C5EA_41CB_8359_78C305F1E83A_.wvu.FilterData">BIM!$A$119:$L$149</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_E033F24B_222D_4C10_9E81_2CD13F2D27CA_.wvu.FilterData">BIM!$A$775:$L$811</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_DC196AA5_A4AE_4C93_995D_C8FA5331B2E2_.wvu.FilterData">BIM!$A$521:$L$531</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_76526F03_6BB6_47C6_A22D_8CED733D2C92_.wvu.FilterData">BIM!$A$429:$L$462</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_4CF85566_B44C_4CE0_B041_FF442715F5FB_.wvu.FilterData">BIM!$A$625:$L$658</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_C3F86223_1CE5_44C1_87CE_40666E8A308F_.wvu.FilterData">BIM!$A$710:$L$724</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_A984F94B_0BB4_4433_89DB_AFDFBD6AE7F9_.wvu.FilterData">BIM!$A$315:$L$334</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_E41D096E_0ABB_48D0_A4ED_16352B60F84D_.wvu.FilterData">BIM!$A$1:$N$1125</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_52071FA0_C79C_4E2C_9B82_5FC05209D4E7_.wvu.FilterData">BIM!$A$770:$L$793</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_98404195_76EE_4140_9039_AD3068CC13E6_.wvu.FilterData">BIM!$A$1009:$L$1031</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_C56FDD5D_C848_4EA9_8EC0_B3E8FFB57F91_.wvu.FilterData">BIM!$A$875:$L$890</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_D8E019AC_D677_4A71_A7A7_F65745991DC9_.wvu.FilterData">BIM!$A$37:$L$69</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_05E28A09_23CF_4F91_95FB_5F959B17C232_.wvu.FilterData">BIM!$A$728:$L$774</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_DE8783DB_61C2_4EA7_A572_E71C0795FEA1_.wvu.FilterData">BIM!$A$994:$L$1005</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_361013E5_E895_48D0_B579_FC88480C5F47_.wvu.FilterData">BIM!$A$794:$L$802</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_D560E911_BF63_4572_BF1B_4AF1C36BB0F6_.wvu.FilterData">BIM!$A$891:$L$1023</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_2CC30FC2_C6C4_4FBA_8A83_09C3EDAFCB1A_.wvu.FilterData">BIM!$A$75:$L$157</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_33596B96_C2AA_4CF3_93FF_CB3D5E438131_.wvu.FilterData">BIM!$A$551:$L$565</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_EB148AC7_BEAD_4132_98AC_E5E0C12786AC_.wvu.FilterData">BIM!$A$562:$L$572</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_578123A8_10D5_4CF4_BC99_156B0063D202_.wvu.FilterData">BIM!$A$803:$L$874</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_88CF1269_A498_4F96_8096_DF9A248D182F_.wvu.FilterData">BIM!$A$533:$L$565</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_0525DDEC_C925_45B1_9847_6B10EECC72E1_.wvu.FilterData">BIM!$A$1039:$L$1074</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_4366E692_EA63_470F_AD6B_F16D89BA7A13_.wvu.FilterData">BIM!$A$119:$L$149</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_29953007_05A1_4AA5_AF83_C71F0162324C_.wvu.FilterData">BIM!$A$718:$L$769</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_4B29C85D_8F4B_41C5_98E1_179F34C547AD_.wvu.FilterData">BIM!$A$832:$L$863</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_30753236_7AA4_4693_B24C_742CAA8C26E5_.wvu.FilterData">BIM!$A$2:$L$36</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_D1D0E9F4_CDA8_4E5B_93DD_F2C29EAD6080_.wvu.FilterData">BIM!$A$970:$L$993</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_85A2FC98_A2B5_4E0D_AA36_AF69AE3B83B5_.wvu.FilterData">BIM!$A$267:$H$314</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_4484A6DE_93A6_4A06_9698_3E212A1F4069_.wvu.FilterData">BIM!$A$1:$O$1125</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_941CA0B9_8F0E_40BD_8E17_11D8E91E25A7_.wvu.FilterData">BIM!$A$923:$L$960</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_191CE3A5_E0F7_4A5A_A27B_B2DCD098BF72_.wvu.FilterData">BIM!$A$144:$L$266</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_1C914825_B774_497B_9951_7424A275C6C8_.wvu.FilterData">BIM!$A$1:$O$1125</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_4900EDE6_BCBD_49E0_843B_3969248BB0EF_.wvu.FilterData">BIM!$A$335:$L$346</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_FB5A0C69_03A9_4211_8A02_EDD5A66544AD_.wvu.FilterData">BIM!$A$573:$L$584</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_986591FF_6F24_4023_8AC1_D53F01184713_.wvu.FilterData">BIM!$A$77:$L$128</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_6FC2398D_0036_45FB_A79D_B7AEBC0EB69B_.wvu.FilterData">BIM!$A$565:$L$574</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_440974C0_07E2_4054_AD03_D6D4230CA7A2_.wvu.FilterData">BIM!$A$573:$L$591</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_18217A88_0981_418C_ABFA_AC931682F80F_.wvu.FilterData">BIM!$A$267:$L$314</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_0B8CAF0B_9853_4166_868E_F5DFCF10FF93_.wvu.FilterData">BIM!$A$1:$O$1125</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{B7D1E82B-A5E5-4C14-9C86-B61A78ED8084}" name="Pekerjaan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{D6318188-C0E0-4364-A149-FD9E8D671A1B}" name="Buah"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{2039A978-ADAF-4711-8B07-046A7AD53BA6}" name="Pakaian"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{F436789B-C5EA-41CB-8359-78C305F1E83A}" name="Makanan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{BE442BB6-3A31-442F-B924-D13D0F598ECC}" name="Kata Penghubung"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{7B44AC12-E6B4-4313-993B-10F7132B892F}" name="Budaya"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{DBDF39FA-7899-4557-B3BC-352C416503A3}" name="Warna"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{3A76F548-2F88-4245-B104-5C766A91C956}" name="Kata Kerja"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{9DF68346-E0CA-4FA3-B5D1-1AD86B191463}" name="Kata Ganti Nama"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{560CED10-97E3-4B8F-9E2D-42501DEDD37A}" name="Haiwan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{48CE27A7-5499-4811-A41E-787093C14E7E}" name="Kata Bantu"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{AABB1EE6-8061-4BBE-83FC-087E9C58414A}" name="Kata Tanya"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{DE900718-0161-4792-8EAB-C58F78F69250}" name="Kerajaan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{9E4183D2-CC5A-4D20-BB9A-2F013C0CE815}" name="Angka"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{9E47DD61-E6DE-488B-80BA-967A50C8AB36}" name="Pengangkutan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{92BEF0B2-FF4A-4089-8EE6-8E4DADA938AF}" name="Tempat - Bangunan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{0ECEE141-0B77-44E5-A6DE-68B5A15450B4}" name="Kesihatan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{49E7F3CE-F40C-4FED-BEF8-26F090EE4EAB}" name="Badan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{C6F25ED8-01F5-4EC6-BA59-11F1B290E9F7}" name="Sukan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{1A8878F0-0412-4D55-9C2F-095CAD9E6CFA}" name="Ucapan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{43C9EAE1-EEE7-465A-B2FE-FCC5D6144576}" name="Masa"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{FAE9710F-D2BA-4EBD-88A7-23B01C8DBCFC}" name="Arah"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{AF68C2CF-34E8-443E-B4ED-BB66CB150D6B}" name="Alam"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{030204D7-095F-4354-969B-56C1AA7143AE}" name="Pertubuhan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{3D296FF4-2091-4F77-BB20-5342594B263E}" name="Agama"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{A856CC1B-B362-4556-ACE2-C976256EBF5B}" name="Komunikasi"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{8BD75489-4874-47F0-8DF3-393379AB259B}" name="Kata Sifat"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{724DC91F-FF1E-468C-B992-B1D0F51CCC52}" name="Filter 4"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{CA698D16-9134-4DB4-984A-29693DB788A8}" name="Filter 2"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{0909C5DC-ED19-4D4A-9DB0-5392CF96C4D4}" name="Negeri"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{EF393267-77E9-4937-B374-A059A55A3DDA}" name="Filter 3"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{EBA9F249-1672-448E-8531-16FD1942FCAD}" name="Perasaan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{8232B643-36E7-487B-B1D6-FD3DA06BF1E9}" name="Pendidikan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{E460850B-B72B-48C4-B246-11D0D04F03F5}" name="Filter 1"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{743AD89C-320C-4C4C-BC5F-7EC0A02EECDE}" name="Kecacatan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{A7B4F8D0-C2B2-4D23-888B-901C02EDA207}" name="Keluarga"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{C330DD12-F7AD-4A16-8E93-F60E7DD26815}" name="Benda"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{D8E7AD2B-1D6A-4A53-BADF-5738E01F788C}" name="Binatang"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{05E28A09-23CF-4F91-95FB-5F959B17C232}" name="Pekerjaan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{52071FA0-C79C-4E2C-9B82-5FC05209D4E7}" name="Buah"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{4CF85566-B44C-4CE0-B041-FF442715F5FB}" name="Pakaian"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{4366E692-EA63-470F-AD6B-F16D89BA7A13}" name="Makanan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{C56FDD5D-C848-4EA9-8EC0-B3E8FFB57F91}" name="Kata Penghubung"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{A984F94B-0BB4-4433-89DB-AFDFBD6AE7F9}" name="Budaya"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{DE8783DB-61C2-4EA7-A572-E71C0795FEA1}" name="Warna"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{578123A8-10D5-4CF4-BC99-156B0063D202}" name="Kata Kerja"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{440974C0-07E2-4054-AD03-D6D4230CA7A2}" name="Kata Ganti Nama"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{85A2FC98-A2B5-4E0D-AA36-AF69AE3B83B5}" name="Haiwan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{361013E5-E895-48D0-B579-FC88480C5F47}" name="Kata Bantu"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{4900EDE6-BCBD-49E0-843B-3969248BB0EF}" name="Kata Tanya"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{98404195-76EE-4140-9039-AD3068CC13E6}" name="Kerajaan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{986591FF-6F24-4023-8AC1-D53F01184713}" name="Angka"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{6FC2398D-0036-45FB-A79D-B7AEBC0EB69B}" name="Pengangkutan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{2CC30FC2-C6C4-4FBA-8A83-09C3EDAFCB1A}" name="Tempat - Bangunan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{76526F03-6BB6-47C6-A22D-8CED733D2C92}" name="Kesihatan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{EB148AC7-BEAD-4132-98AC-E5E0C12786AC}" name="Badan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{941CA0B9-8F0E-40BD-8E17-11D8E91E25A7}" name="Sukan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{D1D0E9F4-CDA8-4E5B-93DD-F2C29EAD6080}" name="Ucapan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{29953007-05A1-4AA5-AF83-C71F0162324C}" name="Masa"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{C3F86223-1CE5-44C1-87CE-40666E8A308F}" name="Arah"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{D8E019AC-D677-4A71-A7A7-F65745991DC9}" name="Alam"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{0525DDEC-C925-45B1-9847-6B10EECC72E1}" name="Pertubuhan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{30753236-7AA4-4693-B24C-742CAA8C26E5}" name="Agama"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{FB5A0C69-03A9-4211-8A02-EDD5A66544AD}" name="Komunikasi"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{D560E911-BF63-4572-BF1B-4AF1C36BB0F6}" name="Kata Sifat"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{0B8CAF0B-9853-4166-868E-F5DFCF10FF93}" name="Filter 4"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{E41D096E-0ABB-48D0-A4ED-16352B60F84D}" name="Filter 2"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{33596B96-C2AA-4CF3-93FF-CB3D5E438131}" name="Negeri"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{4484A6DE-93A6-4A06-9698-3E212A1F4069}" name="Filter 3"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{4B29C85D-8F4B-41C5-98E1-179F34C547AD}" name="Perasaan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{E033F24B-222D-4C10-9E81-2CD13F2D27CA}" name="Pendidikan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{1C914825-B774-497B-9951-7424A275C6C8}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{DC196AA5-A4AE-4C93-995D-C8FA5331B2E2}" name="Kecacatan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{88CF1269-A498-4F96-8096-DF9A248D182F}" name="Keluarga"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{191CE3A5-E0F7-4A5A-A27B-B2DCD098BF72}" name="Benda"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{18217A88-0981-418C-ABFA-AC931682F80F}" name="Binatang"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14782" uniqueCount="3209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14781" uniqueCount="3209">
   <si>
     <t>Perkataan</t>
   </si>
@@ -10496,41 +10496,41 @@
     <t>Toliet</t>
   </si>
   <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Things/Communication</t>
+  </si>
+  <si>
+    <t>Tempat/Pendidikan</t>
+  </si>
+  <si>
+    <t>Places/Education</t>
+  </si>
+  <si>
+    <t>Tempat/Pertubuhan</t>
+  </si>
+  <si>
+    <t>Places/Organisations</t>
+  </si>
+  <si>
+    <t>Tempat/Pengangkutan</t>
+  </si>
+  <si>
+    <t>Places/Transportation</t>
+  </si>
+  <si>
     <t>Isyarat Baru/Isyarat Baru</t>
   </si>
   <si>
     <t>New Signs/New Signs</t>
-  </si>
-  <si>
-    <t>Home</t>
-  </si>
-  <si>
-    <t>Things/Communication</t>
-  </si>
-  <si>
-    <t>Tempat/Pendidikan</t>
-  </si>
-  <si>
-    <t>Places/Education</t>
-  </si>
-  <si>
-    <t>Tempat/Pertubuhan</t>
-  </si>
-  <si>
-    <t>Places/Organisations</t>
-  </si>
-  <si>
-    <t>Tempat/Pengangkutan</t>
-  </si>
-  <si>
-    <t>Places/Transportation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="36">
+  <fonts count="35">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -10706,10 +10706,6 @@
       <color theme="5"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <sz val="11.0"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -10755,7 +10751,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="96">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -11031,9 +11027,6 @@
     </xf>
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="35" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -67551,23 +67544,23 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{49E7F3CE-F40C-4FED-BEF8-26F090EE4EAB}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{EB148AC7-BEAD-4132-98AC-E5E0C12786AC}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$562:$L$572"/>
     </customSheetView>
-    <customSheetView guid="{0ECEE141-0B77-44E5-A6DE-68B5A15450B4}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{76526F03-6BB6-47C6-A22D-8CED733D2C92}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$429:$L$462">
         <sortState ref="A429:L462">
           <sortCondition ref="A429:A462"/>
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{A7B4F8D0-C2B2-4D23-888B-901C02EDA207}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{88CF1269-A498-4F96-8096-DF9A248D182F}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$533:$L$565"/>
     </customSheetView>
-    <customSheetView guid="{743AD89C-320C-4C4C-BC5F-7EC0A02EECDE}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{DC196AA5-A4AE-4C93-995D-C8FA5331B2E2}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$521:$L$531"/>
     </customSheetView>
-    <customSheetView guid="{0909C5DC-ED19-4D4A-9DB0-5392CF96C4D4}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{33596B96-C2AA-4CF3-93FF-CB3D5E438131}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$551:$L$565">
         <filterColumn colId="6">
           <filters>
@@ -67579,14 +67572,14 @@
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{F436789B-C5EA-41CB-8359-78C305F1E83A}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{4366E692-EA63-470F-AD6B-F16D89BA7A13}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$119:$L$149">
         <sortState ref="A119:L149">
           <sortCondition ref="A119:A149"/>
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{CA698D16-9134-4DB4-984A-29693DB788A8}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{E41D096E-0ABB-48D0-A4ED-16352B60F84D}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$N$1125">
         <filterColumn colId="13">
           <filters>
@@ -67595,20 +67588,20 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{8BD75489-4874-47F0-8DF3-393379AB259B}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{D560E911-BF63-4572-BF1B-4AF1C36BB0F6}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$891:$L$1023"/>
     </customSheetView>
-    <customSheetView guid="{AF68C2CF-34E8-443E-B4ED-BB66CB150D6B}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{D8E019AC-D677-4A71-A7A7-F65745991DC9}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$37:$L$69"/>
     </customSheetView>
-    <customSheetView guid="{92BEF0B2-FF4A-4089-8EE6-8E4DADA938AF}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{2CC30FC2-C6C4-4FBA-8A83-09C3EDAFCB1A}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$75:$L$157">
         <sortState ref="A75:L157">
           <sortCondition ref="A75:A157"/>
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{3D296FF4-2091-4F77-BB20-5342594B263E}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{30753236-7AA4-4693-B24C-742CAA8C26E5}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$2:$L$36">
         <filterColumn colId="6">
           <filters>
@@ -67617,13 +67610,13 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{1A8878F0-0412-4D55-9C2F-095CAD9E6CFA}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{D1D0E9F4-CDA8-4E5B-93DD-F2C29EAD6080}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$970:$L$993"/>
     </customSheetView>
-    <customSheetView guid="{AABB1EE6-8061-4BBE-83FC-087E9C58414A}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{4900EDE6-BCBD-49E0-843B-3969248BB0EF}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$335:$L$346"/>
     </customSheetView>
-    <customSheetView guid="{43C9EAE1-EEE7-465A-B2FE-FCC5D6144576}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{29953007-05A1-4AA5-AF83-C71F0162324C}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$718:$L$769">
         <filterColumn colId="4">
           <filters>
@@ -67636,35 +67629,35 @@
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{D6318188-C0E0-4364-A149-FD9E8D671A1B}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{52071FA0-C79C-4E2C-9B82-5FC05209D4E7}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$770:$L$793"/>
     </customSheetView>
-    <customSheetView guid="{DE900718-0161-4792-8EAB-C58F78F69250}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{98404195-76EE-4140-9039-AD3068CC13E6}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1009:$L$1031"/>
     </customSheetView>
-    <customSheetView guid="{FAE9710F-D2BA-4EBD-88A7-23B01C8DBCFC}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{C3F86223-1CE5-44C1-87CE-40666E8A308F}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$710:$L$724"/>
     </customSheetView>
-    <customSheetView guid="{030204D7-095F-4354-969B-56C1AA7143AE}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{0525DDEC-C925-45B1-9847-6B10EECC72E1}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1039:$L$1074"/>
     </customSheetView>
-    <customSheetView guid="{EBA9F249-1672-448E-8531-16FD1942FCAD}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{4B29C85D-8F4B-41C5-98E1-179F34C547AD}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$832:$L$863"/>
     </customSheetView>
-    <customSheetView guid="{8232B643-36E7-487B-B1D6-FD3DA06BF1E9}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{E033F24B-222D-4C10-9E81-2CD13F2D27CA}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$775:$L$811">
         <sortState ref="A775:L811">
           <sortCondition ref="A775:A811"/>
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{3A76F548-2F88-4245-B104-5C766A91C956}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{578123A8-10D5-4CF4-BC99-156B0063D202}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$803:$L$874"/>
     </customSheetView>
-    <customSheetView guid="{A856CC1B-B362-4556-ACE2-C976256EBF5B}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{FB5A0C69-03A9-4211-8A02-EDD5A66544AD}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$573:$L$584"/>
     </customSheetView>
-    <customSheetView guid="{B7D1E82B-A5E5-4C14-9C86-B61A78ED8084}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{05E28A09-23CF-4F91-95FB-5F959B17C232}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$728:$L$774">
         <filterColumn colId="6">
           <filters>
@@ -67676,24 +67669,24 @@
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{560CED10-97E3-4B8F-9E2D-42501DEDD37A}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{85A2FC98-A2B5-4E0D-AA36-AF69AE3B83B5}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$267:$H$314">
         <sortState ref="A267:H314">
           <sortCondition ref="A267:A314"/>
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{9E47DD61-E6DE-488B-80BA-967A50C8AB36}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{6FC2398D-0036-45FB-A79D-B7AEBC0EB69B}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$565:$L$574">
         <sortState ref="A565:L574">
           <sortCondition ref="A565:A574"/>
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{BE442BB6-3A31-442F-B924-D13D0F598ECC}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{C56FDD5D-C848-4EA9-8EC0-B3E8FFB57F91}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$875:$L$890"/>
     </customSheetView>
-    <customSheetView guid="{C330DD12-F7AD-4A16-8E93-F60E7DD26815}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{191CE3A5-E0F7-4A5A-A27B-B2DCD098BF72}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$144:$L$266">
         <filterColumn colId="11">
           <filters>
@@ -67705,10 +67698,10 @@
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{48CE27A7-5499-4811-A41E-787093C14E7E}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{361013E5-E895-48D0-B579-FC88480C5F47}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$794:$L$802"/>
     </customSheetView>
-    <customSheetView guid="{724DC91F-FF1E-468C-B992-B1D0F51CCC52}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{0B8CAF0B-9853-4166-868E-F5DFCF10FF93}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$O$1125">
         <filterColumn colId="2">
           <filters>
@@ -67726,7 +67719,7 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{EF393267-77E9-4937-B374-A059A55A3DDA}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{4484A6DE-93A6-4A06-9698-3E212A1F4069}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$O$1125">
         <filterColumn colId="13">
           <filters>
@@ -67735,36 +67728,36 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{E460850B-B72B-48C4-B246-11D0D04F03F5}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{1C914825-B774-497B-9951-7424A275C6C8}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$O$1125"/>
     </customSheetView>
-    <customSheetView guid="{9E4183D2-CC5A-4D20-BB9A-2F013C0CE815}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{986591FF-6F24-4023-8AC1-D53F01184713}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$77:$L$128"/>
     </customSheetView>
-    <customSheetView guid="{7B44AC12-E6B4-4313-993B-10F7132B892F}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{A984F94B-0BB4-4433-89DB-AFDFBD6AE7F9}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$315:$L$334">
         <sortState ref="A315:L334">
           <sortCondition ref="A315:A334"/>
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{9DF68346-E0CA-4FA3-B5D1-1AD86B191463}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{440974C0-07E2-4054-AD03-D6D4230CA7A2}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$573:$L$591"/>
     </customSheetView>
-    <customSheetView guid="{2039A978-ADAF-4711-8B07-046A7AD53BA6}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{4CF85566-B44C-4CE0-B041-FF442715F5FB}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$625:$L$658"/>
     </customSheetView>
-    <customSheetView guid="{C6F25ED8-01F5-4EC6-BA59-11F1B290E9F7}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{941CA0B9-8F0E-40BD-8E17-11D8E91E25A7}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$923:$L$960">
         <sortState ref="A923:L960">
           <sortCondition ref="A923:A960"/>
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{DBDF39FA-7899-4557-B3BC-352C416503A3}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{DE8783DB-61C2-4EA7-A572-E71C0795FEA1}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$994:$L$1005"/>
     </customSheetView>
-    <customSheetView guid="{D8E7AD2B-1D6A-4A53-BADF-5738E01F788C}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{18217A88-0981-418C-ABFA-AC931682F80F}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$267:$L$314"/>
     </customSheetView>
   </customSheetViews>
@@ -67779,11 +67772,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
+    <dataValidation type="list" allowBlank="1" sqref="D2:D1580">
+      <formula1>Group!$B$2:$B1580</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="C2:C1580">
-      <formula1>Group!$A$3:$A1580</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D2:D1580">
-      <formula1>Group!$B$3:$B1580</formula1>
+      <formula1>Group!$A$2:$A1580</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J2:J1580">
       <formula1>"Yes,No"</formula1>
@@ -68669,428 +68662,426 @@
     </row>
     <row r="2">
       <c r="A2" s="92" t="s">
-        <v>3199</v>
+        <v>1321</v>
       </c>
       <c r="B2" s="92" t="s">
-        <v>3200</v>
-      </c>
-      <c r="C2" s="92" t="s">
-        <v>3201</v>
-      </c>
+        <v>1322</v>
+      </c>
+      <c r="C2" s="92"/>
     </row>
     <row r="3">
       <c r="A3" s="93" t="s">
-        <v>1321</v>
+        <v>1418</v>
       </c>
       <c r="B3" s="93" t="s">
-        <v>1322</v>
+        <v>1419</v>
       </c>
       <c r="C3" s="93"/>
     </row>
     <row r="4">
-      <c r="A4" s="94" t="s">
-        <v>1418</v>
+      <c r="A4" s="92" t="s">
+        <v>16</v>
       </c>
       <c r="B4" s="94" t="s">
-        <v>1419</v>
-      </c>
-      <c r="C4" s="94"/>
+        <v>17</v>
+      </c>
+      <c r="C4" s="92" t="s">
+        <v>3199</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="93" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="B5" s="95" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="C5" s="93" t="s">
-        <v>3201</v>
+        <v>3199</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="94" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="96" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" s="94" t="s">
-        <v>3201</v>
+      <c r="A6" s="92" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6" s="94" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" s="92" t="s">
+        <v>3199</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="93" t="s">
-        <v>167</v>
-      </c>
-      <c r="B7" s="95" t="s">
-        <v>168</v>
-      </c>
-      <c r="C7" s="93" t="s">
-        <v>3201</v>
-      </c>
+        <v>1616</v>
+      </c>
+      <c r="B7" s="93" t="s">
+        <v>1617</v>
+      </c>
+      <c r="C7" s="93"/>
     </row>
     <row r="8">
-      <c r="A8" s="94" t="s">
-        <v>1616</v>
+      <c r="A8" s="92" t="s">
+        <v>1769</v>
       </c>
       <c r="B8" s="94" t="s">
-        <v>1617</v>
-      </c>
-      <c r="C8" s="94"/>
+        <v>3200</v>
+      </c>
+      <c r="C8" s="92"/>
     </row>
     <row r="9">
       <c r="A9" s="93" t="s">
-        <v>1769</v>
-      </c>
-      <c r="B9" s="95" t="s">
-        <v>3202</v>
+        <v>1804</v>
+      </c>
+      <c r="B9" s="93" t="s">
+        <v>1805</v>
       </c>
       <c r="C9" s="93"/>
     </row>
     <row r="10">
-      <c r="A10" s="94" t="s">
-        <v>1804</v>
-      </c>
-      <c r="B10" s="94" t="s">
-        <v>1805</v>
-      </c>
-      <c r="C10" s="94"/>
+      <c r="A10" s="92" t="s">
+        <v>1901</v>
+      </c>
+      <c r="B10" s="92" t="s">
+        <v>1902</v>
+      </c>
+      <c r="C10" s="92"/>
     </row>
     <row r="11">
       <c r="A11" s="93" t="s">
-        <v>1901</v>
+        <v>1953</v>
       </c>
       <c r="B11" s="93" t="s">
-        <v>1902</v>
+        <v>1954</v>
       </c>
       <c r="C11" s="93"/>
     </row>
     <row r="12">
-      <c r="A12" s="94" t="s">
-        <v>1953</v>
-      </c>
-      <c r="B12" s="94" t="s">
-        <v>1954</v>
-      </c>
-      <c r="C12" s="94"/>
+      <c r="A12" s="92" t="s">
+        <v>2060</v>
+      </c>
+      <c r="B12" s="92" t="s">
+        <v>2061</v>
+      </c>
+      <c r="C12" s="92"/>
     </row>
     <row r="13">
       <c r="A13" s="93" t="s">
-        <v>2060</v>
+        <v>2100</v>
       </c>
       <c r="B13" s="93" t="s">
-        <v>2061</v>
+        <v>2101</v>
       </c>
       <c r="C13" s="93"/>
     </row>
     <row r="14">
-      <c r="A14" s="94" t="s">
-        <v>2100</v>
-      </c>
-      <c r="B14" s="94" t="s">
-        <v>2101</v>
-      </c>
-      <c r="C14" s="94"/>
+      <c r="A14" s="92" t="s">
+        <v>2172</v>
+      </c>
+      <c r="B14" s="92" t="s">
+        <v>2173</v>
+      </c>
+      <c r="C14" s="92" t="s">
+        <v>3199</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="93" t="s">
-        <v>2172</v>
+        <v>2323</v>
       </c>
       <c r="B15" s="93" t="s">
-        <v>2173</v>
+        <v>2324</v>
       </c>
       <c r="C15" s="93" t="s">
-        <v>3201</v>
+        <v>3199</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="94" t="s">
-        <v>2323</v>
-      </c>
-      <c r="B16" s="94" t="s">
-        <v>2324</v>
-      </c>
-      <c r="C16" s="94" t="s">
-        <v>3201</v>
+      <c r="A16" s="92" t="s">
+        <v>2721</v>
+      </c>
+      <c r="B16" s="92" t="s">
+        <v>2722</v>
+      </c>
+      <c r="C16" s="92" t="s">
+        <v>3199</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="93" t="s">
-        <v>2721</v>
+        <v>206</v>
       </c>
       <c r="B17" s="93" t="s">
-        <v>2722</v>
+        <v>207</v>
       </c>
       <c r="C17" s="93" t="s">
-        <v>3201</v>
+        <v>3199</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="94" t="s">
-        <v>206</v>
-      </c>
-      <c r="B18" s="94" t="s">
-        <v>207</v>
-      </c>
-      <c r="C18" s="94" t="s">
-        <v>3201</v>
+      <c r="A18" s="92" t="s">
+        <v>238</v>
+      </c>
+      <c r="B18" s="92" t="s">
+        <v>239</v>
+      </c>
+      <c r="C18" s="92" t="s">
+        <v>3199</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="93" t="s">
-        <v>238</v>
-      </c>
-      <c r="B19" s="93" t="s">
-        <v>239</v>
+        <v>308</v>
+      </c>
+      <c r="B19" s="95" t="s">
+        <v>309</v>
       </c>
       <c r="C19" s="93" t="s">
-        <v>3201</v>
+        <v>3199</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="94" t="s">
-        <v>308</v>
-      </c>
-      <c r="B20" s="96" t="s">
-        <v>309</v>
-      </c>
-      <c r="C20" s="94" t="s">
-        <v>3201</v>
+      <c r="A20" s="92" t="s">
+        <v>2770</v>
+      </c>
+      <c r="B20" s="92" t="s">
+        <v>2771</v>
+      </c>
+      <c r="C20" s="92" t="s">
+        <v>3199</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="93" t="s">
-        <v>2770</v>
+        <v>407</v>
       </c>
       <c r="B21" s="93" t="s">
-        <v>2771</v>
-      </c>
-      <c r="C21" s="93" t="s">
-        <v>3201</v>
-      </c>
+        <v>408</v>
+      </c>
+      <c r="C21" s="93"/>
     </row>
     <row r="22">
-      <c r="A22" s="94" t="s">
-        <v>407</v>
-      </c>
-      <c r="B22" s="94" t="s">
-        <v>408</v>
-      </c>
-      <c r="C22" s="94"/>
+      <c r="A22" s="92" t="s">
+        <v>2826</v>
+      </c>
+      <c r="B22" s="92" t="s">
+        <v>2827</v>
+      </c>
+      <c r="C22" s="92"/>
     </row>
     <row r="23">
       <c r="A23" s="93" t="s">
-        <v>2826</v>
+        <v>2927</v>
       </c>
       <c r="B23" s="93" t="s">
-        <v>2827</v>
+        <v>2928</v>
       </c>
       <c r="C23" s="93"/>
     </row>
     <row r="24">
-      <c r="A24" s="94" t="s">
-        <v>2927</v>
-      </c>
-      <c r="B24" s="94" t="s">
-        <v>2928</v>
-      </c>
-      <c r="C24" s="94"/>
+      <c r="A24" s="92" t="s">
+        <v>463</v>
+      </c>
+      <c r="B24" s="92" t="s">
+        <v>464</v>
+      </c>
+      <c r="C24" s="92"/>
     </row>
     <row r="25">
       <c r="A25" s="93" t="s">
-        <v>463</v>
+        <v>587</v>
       </c>
       <c r="B25" s="93" t="s">
-        <v>464</v>
+        <v>588</v>
       </c>
       <c r="C25" s="93"/>
     </row>
     <row r="26">
-      <c r="A26" s="94" t="s">
-        <v>587</v>
-      </c>
-      <c r="B26" s="94" t="s">
-        <v>588</v>
-      </c>
-      <c r="C26" s="94"/>
+      <c r="A26" s="92" t="s">
+        <v>563</v>
+      </c>
+      <c r="B26" s="92" t="s">
+        <v>564</v>
+      </c>
+      <c r="C26" s="92"/>
     </row>
     <row r="27">
       <c r="A27" s="93" t="s">
-        <v>563</v>
+        <v>641</v>
       </c>
       <c r="B27" s="93" t="s">
-        <v>564</v>
+        <v>642</v>
       </c>
       <c r="C27" s="93"/>
     </row>
     <row r="28">
       <c r="A28" s="94" t="s">
-        <v>641</v>
+        <v>726</v>
       </c>
       <c r="B28" s="94" t="s">
-        <v>642</v>
-      </c>
-      <c r="C28" s="94"/>
+        <v>727</v>
+      </c>
+      <c r="C28" s="92"/>
     </row>
     <row r="29">
-      <c r="A29" s="95" t="s">
-        <v>726</v>
-      </c>
-      <c r="B29" s="95" t="s">
-        <v>727</v>
+      <c r="A29" s="93" t="s">
+        <v>603</v>
+      </c>
+      <c r="B29" s="93" t="s">
+        <v>604</v>
       </c>
       <c r="C29" s="93"/>
     </row>
     <row r="30">
-      <c r="A30" s="94" t="s">
-        <v>603</v>
-      </c>
-      <c r="B30" s="94" t="s">
-        <v>604</v>
-      </c>
-      <c r="C30" s="94"/>
+      <c r="A30" s="92" t="s">
+        <v>749</v>
+      </c>
+      <c r="B30" s="92" t="s">
+        <v>750</v>
+      </c>
+      <c r="C30" s="92" t="s">
+        <v>3199</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="93" t="s">
-        <v>749</v>
+        <v>814</v>
       </c>
       <c r="B31" s="93" t="s">
-        <v>750</v>
+        <v>815</v>
       </c>
       <c r="C31" s="93" t="s">
-        <v>3201</v>
+        <v>3199</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="94" t="s">
-        <v>814</v>
-      </c>
-      <c r="B32" s="94" t="s">
-        <v>815</v>
-      </c>
-      <c r="C32" s="94" t="s">
-        <v>3201</v>
+      <c r="A32" s="92" t="s">
+        <v>2989</v>
+      </c>
+      <c r="B32" s="92" t="s">
+        <v>2990</v>
+      </c>
+      <c r="C32" s="92" t="s">
+        <v>3199</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="93" t="s">
-        <v>2989</v>
+        <v>869</v>
       </c>
       <c r="B33" s="93" t="s">
-        <v>2990</v>
+        <v>870</v>
       </c>
       <c r="C33" s="93" t="s">
-        <v>3201</v>
+        <v>3199</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="94" t="s">
-        <v>869</v>
-      </c>
-      <c r="B34" s="94" t="s">
-        <v>870</v>
-      </c>
-      <c r="C34" s="94" t="s">
-        <v>3201</v>
+      <c r="A34" s="92" t="s">
+        <v>3010</v>
+      </c>
+      <c r="B34" s="92" t="s">
+        <v>3011</v>
+      </c>
+      <c r="C34" s="92" t="s">
+        <v>3199</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="93" t="s">
-        <v>3010</v>
+        <v>981</v>
       </c>
       <c r="B35" s="93" t="s">
-        <v>3011</v>
+        <v>982</v>
       </c>
       <c r="C35" s="93" t="s">
-        <v>3201</v>
+        <v>3199</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="94" t="s">
-        <v>981</v>
-      </c>
-      <c r="B36" s="94" t="s">
-        <v>982</v>
-      </c>
-      <c r="C36" s="94" t="s">
-        <v>3201</v>
+      <c r="A36" s="92" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B36" s="92" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C36" s="92" t="s">
+        <v>3199</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="93" t="s">
-        <v>1081</v>
+        <v>3054</v>
       </c>
       <c r="B37" s="93" t="s">
-        <v>1082</v>
+        <v>3055</v>
       </c>
       <c r="C37" s="93" t="s">
-        <v>3201</v>
+        <v>3199</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="94" t="s">
-        <v>3054</v>
-      </c>
-      <c r="B38" s="94" t="s">
-        <v>3055</v>
-      </c>
-      <c r="C38" s="94" t="s">
-        <v>3201</v>
-      </c>
+      <c r="A38" s="92" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B38" s="92" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C38" s="92"/>
     </row>
     <row r="39">
       <c r="A39" s="93" t="s">
-        <v>1102</v>
+        <v>3074</v>
       </c>
       <c r="B39" s="93" t="s">
-        <v>1103</v>
+        <v>3075</v>
       </c>
       <c r="C39" s="93"/>
     </row>
     <row r="40">
-      <c r="A40" s="94" t="s">
-        <v>3074</v>
-      </c>
-      <c r="B40" s="94" t="s">
-        <v>3075</v>
-      </c>
-      <c r="C40" s="94"/>
+      <c r="A40" s="92" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B40" s="92" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C40" s="92"/>
     </row>
     <row r="41">
       <c r="A41" s="93" t="s">
-        <v>1133</v>
+        <v>1172</v>
       </c>
       <c r="B41" s="93" t="s">
-        <v>1134</v>
+        <v>1173</v>
       </c>
       <c r="C41" s="93"/>
     </row>
     <row r="42">
-      <c r="A42" s="94" t="s">
-        <v>1172</v>
-      </c>
-      <c r="B42" s="94" t="s">
-        <v>1173</v>
-      </c>
-      <c r="C42" s="94"/>
+      <c r="A42" s="92" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B42" s="92" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C42" s="92"/>
     </row>
     <row r="43">
       <c r="A43" s="93" t="s">
-        <v>1244</v>
+        <v>3109</v>
       </c>
       <c r="B43" s="93" t="s">
-        <v>1245</v>
+        <v>3110</v>
       </c>
       <c r="C43" s="93"/>
     </row>
     <row r="44">
-      <c r="A44" s="94" t="s">
-        <v>3109</v>
-      </c>
-      <c r="B44" s="94" t="s">
-        <v>3110</v>
-      </c>
-      <c r="C44" s="94"/>
+      <c r="A44" s="92" t="s">
+        <v>3201</v>
+      </c>
+      <c r="B44" s="92" t="s">
+        <v>3202</v>
+      </c>
+      <c r="C44" s="92"/>
     </row>
     <row r="45">
       <c r="A45" s="93" t="s">
@@ -69102,31 +69093,31 @@
       <c r="C45" s="93"/>
     </row>
     <row r="46">
-      <c r="A46" s="94" t="s">
+      <c r="A46" s="92" t="s">
         <v>3205</v>
       </c>
-      <c r="B46" s="94" t="s">
+      <c r="B46" s="92" t="s">
         <v>3206</v>
       </c>
-      <c r="C46" s="94"/>
+      <c r="C46" s="92"/>
     </row>
     <row r="47">
       <c r="A47" s="93" t="s">
+        <v>3143</v>
+      </c>
+      <c r="B47" s="93" t="s">
+        <v>3144</v>
+      </c>
+      <c r="C47" s="93"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="95" t="s">
         <v>3207</v>
       </c>
-      <c r="B47" s="93" t="s">
+      <c r="B48" s="95" t="s">
         <v>3208</v>
       </c>
-      <c r="C47" s="93"/>
-    </row>
-    <row r="48">
-      <c r="A48" s="94" t="s">
-        <v>3143</v>
-      </c>
-      <c r="B48" s="94" t="s">
-        <v>3144</v>
-      </c>
-      <c r="C48" s="94"/>
+      <c r="C48" s="95"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Release v1.0.5 UAT (#55)
* added a special category - 'New Signs' in home page, categories page

* Remove dropdowns. And reposition category

* added a special category - 'New Signs' in home page, categories page

* Remove dropdowns. And reposition category

* Solve merge conflicts

* update BIM file

* R1 - Cosmetic - Translate Button Incorrect Render on First Time Landing (#54)

Co-authored-by: Wai Hoe Sin <wsin@guidewire.com>
Co-authored-by: sinwaihoe-gw <85343933+sinwaihoe-gw@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/public/assets/BIM.xlsx
+++ b/public/assets/BIM.xlsx
@@ -7,91 +7,91 @@
     <sheet state="visible" name="Group" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_E033F24B_222D_4C10_9E81_2CD13F2D27CA_.wvu.FilterData">BIM!$A$775:$L$811</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_DC196AA5_A4AE_4C93_995D_C8FA5331B2E2_.wvu.FilterData">BIM!$A$521:$L$531</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_76526F03_6BB6_47C6_A22D_8CED733D2C92_.wvu.FilterData">BIM!$A$429:$L$462</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_4CF85566_B44C_4CE0_B041_FF442715F5FB_.wvu.FilterData">BIM!$A$625:$L$658</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_C3F86223_1CE5_44C1_87CE_40666E8A308F_.wvu.FilterData">BIM!$A$710:$L$724</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_A984F94B_0BB4_4433_89DB_AFDFBD6AE7F9_.wvu.FilterData">BIM!$A$315:$L$334</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_E41D096E_0ABB_48D0_A4ED_16352B60F84D_.wvu.FilterData">BIM!$A$1:$N$1125</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_52071FA0_C79C_4E2C_9B82_5FC05209D4E7_.wvu.FilterData">BIM!$A$770:$L$793</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_98404195_76EE_4140_9039_AD3068CC13E6_.wvu.FilterData">BIM!$A$1009:$L$1031</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_C56FDD5D_C848_4EA9_8EC0_B3E8FFB57F91_.wvu.FilterData">BIM!$A$875:$L$890</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_D8E019AC_D677_4A71_A7A7_F65745991DC9_.wvu.FilterData">BIM!$A$37:$L$69</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_05E28A09_23CF_4F91_95FB_5F959B17C232_.wvu.FilterData">BIM!$A$728:$L$774</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_DE8783DB_61C2_4EA7_A572_E71C0795FEA1_.wvu.FilterData">BIM!$A$994:$L$1005</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_361013E5_E895_48D0_B579_FC88480C5F47_.wvu.FilterData">BIM!$A$794:$L$802</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_D560E911_BF63_4572_BF1B_4AF1C36BB0F6_.wvu.FilterData">BIM!$A$891:$L$1023</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_2CC30FC2_C6C4_4FBA_8A83_09C3EDAFCB1A_.wvu.FilterData">BIM!$A$75:$L$157</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_33596B96_C2AA_4CF3_93FF_CB3D5E438131_.wvu.FilterData">BIM!$A$551:$L$565</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_EB148AC7_BEAD_4132_98AC_E5E0C12786AC_.wvu.FilterData">BIM!$A$562:$L$572</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_578123A8_10D5_4CF4_BC99_156B0063D202_.wvu.FilterData">BIM!$A$803:$L$874</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_88CF1269_A498_4F96_8096_DF9A248D182F_.wvu.FilterData">BIM!$A$533:$L$565</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_0525DDEC_C925_45B1_9847_6B10EECC72E1_.wvu.FilterData">BIM!$A$1039:$L$1074</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_4366E692_EA63_470F_AD6B_F16D89BA7A13_.wvu.FilterData">BIM!$A$119:$L$149</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_29953007_05A1_4AA5_AF83_C71F0162324C_.wvu.FilterData">BIM!$A$718:$L$769</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_4B29C85D_8F4B_41C5_98E1_179F34C547AD_.wvu.FilterData">BIM!$A$832:$L$863</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_30753236_7AA4_4693_B24C_742CAA8C26E5_.wvu.FilterData">BIM!$A$2:$L$36</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_D1D0E9F4_CDA8_4E5B_93DD_F2C29EAD6080_.wvu.FilterData">BIM!$A$970:$L$993</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_85A2FC98_A2B5_4E0D_AA36_AF69AE3B83B5_.wvu.FilterData">BIM!$A$267:$H$314</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_4484A6DE_93A6_4A06_9698_3E212A1F4069_.wvu.FilterData">BIM!$A$1:$O$1125</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_941CA0B9_8F0E_40BD_8E17_11D8E91E25A7_.wvu.FilterData">BIM!$A$923:$L$960</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_191CE3A5_E0F7_4A5A_A27B_B2DCD098BF72_.wvu.FilterData">BIM!$A$144:$L$266</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_1C914825_B774_497B_9951_7424A275C6C8_.wvu.FilterData">BIM!$A$1:$O$1125</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_4900EDE6_BCBD_49E0_843B_3969248BB0EF_.wvu.FilterData">BIM!$A$335:$L$346</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_FB5A0C69_03A9_4211_8A02_EDD5A66544AD_.wvu.FilterData">BIM!$A$573:$L$584</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_986591FF_6F24_4023_8AC1_D53F01184713_.wvu.FilterData">BIM!$A$77:$L$128</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_6FC2398D_0036_45FB_A79D_B7AEBC0EB69B_.wvu.FilterData">BIM!$A$565:$L$574</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_440974C0_07E2_4054_AD03_D6D4230CA7A2_.wvu.FilterData">BIM!$A$573:$L$591</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_18217A88_0981_418C_ABFA_AC931682F80F_.wvu.FilterData">BIM!$A$267:$L$314</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_0B8CAF0B_9853_4166_868E_F5DFCF10FF93_.wvu.FilterData">BIM!$A$1:$O$1125</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_49E7F3CE_F40C_4FED_BEF8_26F090EE4EAB_.wvu.FilterData">BIM!$A$562:$L$572</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_724DC91F_FF1E_468C_B992_B1D0F51CCC52_.wvu.FilterData">BIM!$A$1:$O$1125</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_8232B643_36E7_487B_B1D6_FD3DA06BF1E9_.wvu.FilterData">BIM!$A$775:$L$811</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_8BD75489_4874_47F0_8DF3_393379AB259B_.wvu.FilterData">BIM!$A$891:$L$1023</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_A856CC1B_B362_4556_ACE2_C976256EBF5B_.wvu.FilterData">BIM!$A$573:$L$584</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_DBDF39FA_7899_4557_B3BC_352C416503A3_.wvu.FilterData">BIM!$A$994:$L$1005</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_9E47DD61_E6DE_488B_80BA_967A50C8AB36_.wvu.FilterData">BIM!$A$565:$L$574</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_BE442BB6_3A31_442F_B924_D13D0F598ECC_.wvu.FilterData">BIM!$A$875:$L$890</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_DE900718_0161_4792_8EAB_C58F78F69250_.wvu.FilterData">BIM!$A$1009:$L$1031</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_030204D7_095F_4354_969B_56C1AA7143AE_.wvu.FilterData">BIM!$A$1039:$L$1074</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_D8E7AD2B_1D6A_4A53_BADF_5738E01F788C_.wvu.FilterData">BIM!$A$267:$L$314</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_7B44AC12_E6B4_4313_993B_10F7132B892F_.wvu.FilterData">BIM!$A$315:$L$334</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_AF68C2CF_34E8_443E_B4ED_BB66CB150D6B_.wvu.FilterData">BIM!$A$37:$L$69</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_CA698D16_9134_4DB4_984A_29693DB788A8_.wvu.FilterData">BIM!$A$1:$N$1125</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_743AD89C_320C_4C4C_BC5F_7EC0A02EECDE_.wvu.FilterData">BIM!$A$521:$L$531</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_A7B4F8D0_C2B2_4D23_888B_901C02EDA207_.wvu.FilterData">BIM!$A$533:$L$565</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_43C9EAE1_EEE7_465A_B2FE_FCC5D6144576_.wvu.FilterData">BIM!$A$718:$L$769</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_D6318188_C0E0_4364_A149_FD9E8D671A1B_.wvu.FilterData">BIM!$A$770:$L$793</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_2039A978_ADAF_4711_8B07_046A7AD53BA6_.wvu.FilterData">BIM!$A$625:$L$658</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_C6F25ED8_01F5_4EC6_BA59_11F1B290E9F7_.wvu.FilterData">BIM!$A$923:$L$960</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_3D296FF4_2091_4F77_BB20_5342594B263E_.wvu.FilterData">BIM!$A$2:$L$36</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_560CED10_97E3_4B8F_9E2D_42501DEDD37A_.wvu.FilterData">BIM!$A$267:$H$314</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_FAE9710F_D2BA_4EBD_88A7_23B01C8DBCFC_.wvu.FilterData">BIM!$A$710:$L$724</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_C330DD12_F7AD_4A16_8E93_F60E7DD26815_.wvu.FilterData">BIM!$A$144:$L$266</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_EF393267_77E9_4937_B374_A059A55A3DDA_.wvu.FilterData">BIM!$A$1:$O$1125</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_3A76F548_2F88_4245_B104_5C766A91C956_.wvu.FilterData">BIM!$A$803:$L$874</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_9DF68346_E0CA_4FA3_B5D1_1AD86B191463_.wvu.FilterData">BIM!$A$573:$L$591</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_1A8878F0_0412_4D55_9C2F_095CAD9E6CFA_.wvu.FilterData">BIM!$A$970:$L$993</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_0ECEE141_0B77_44E5_A6DE_68B5A15450B4_.wvu.FilterData">BIM!$A$429:$L$462</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_AABB1EE6_8061_4BBE_83FC_087E9C58414A_.wvu.FilterData">BIM!$A$335:$L$346</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_EBA9F249_1672_448E_8531_16FD1942FCAD_.wvu.FilterData">BIM!$A$832:$L$863</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_B7D1E82B_A5E5_4C14_9C86_B61A78ED8084_.wvu.FilterData">BIM!$A$728:$L$774</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_48CE27A7_5499_4811_A41E_787093C14E7E_.wvu.FilterData">BIM!$A$794:$L$802</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_E460850B_B72B_48C4_B246_11D0D04F03F5_.wvu.FilterData">BIM!$A$1:$O$1125</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_92BEF0B2_FF4A_4089_8EE6_8E4DADA938AF_.wvu.FilterData">BIM!$A$75:$L$157</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_9E4183D2_CC5A_4D20_BB9A_2F013C0CE815_.wvu.FilterData">BIM!$A$77:$L$128</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_0909C5DC_ED19_4D4A_9DB0_5392CF96C4D4_.wvu.FilterData">BIM!$A$551:$L$565</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_F436789B_C5EA_41CB_8359_78C305F1E83A_.wvu.FilterData">BIM!$A$119:$L$149</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{05E28A09-23CF-4F91-95FB-5F959B17C232}" name="Pekerjaan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{52071FA0-C79C-4E2C-9B82-5FC05209D4E7}" name="Buah"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{4CF85566-B44C-4CE0-B041-FF442715F5FB}" name="Pakaian"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{4366E692-EA63-470F-AD6B-F16D89BA7A13}" name="Makanan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{C56FDD5D-C848-4EA9-8EC0-B3E8FFB57F91}" name="Kata Penghubung"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{A984F94B-0BB4-4433-89DB-AFDFBD6AE7F9}" name="Budaya"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{DE8783DB-61C2-4EA7-A572-E71C0795FEA1}" name="Warna"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{578123A8-10D5-4CF4-BC99-156B0063D202}" name="Kata Kerja"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{440974C0-07E2-4054-AD03-D6D4230CA7A2}" name="Kata Ganti Nama"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{85A2FC98-A2B5-4E0D-AA36-AF69AE3B83B5}" name="Haiwan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{361013E5-E895-48D0-B579-FC88480C5F47}" name="Kata Bantu"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{4900EDE6-BCBD-49E0-843B-3969248BB0EF}" name="Kata Tanya"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{98404195-76EE-4140-9039-AD3068CC13E6}" name="Kerajaan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{986591FF-6F24-4023-8AC1-D53F01184713}" name="Angka"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{6FC2398D-0036-45FB-A79D-B7AEBC0EB69B}" name="Pengangkutan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{2CC30FC2-C6C4-4FBA-8A83-09C3EDAFCB1A}" name="Tempat - Bangunan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{76526F03-6BB6-47C6-A22D-8CED733D2C92}" name="Kesihatan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{EB148AC7-BEAD-4132-98AC-E5E0C12786AC}" name="Badan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{941CA0B9-8F0E-40BD-8E17-11D8E91E25A7}" name="Sukan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{D1D0E9F4-CDA8-4E5B-93DD-F2C29EAD6080}" name="Ucapan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{29953007-05A1-4AA5-AF83-C71F0162324C}" name="Masa"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{C3F86223-1CE5-44C1-87CE-40666E8A308F}" name="Arah"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{D8E019AC-D677-4A71-A7A7-F65745991DC9}" name="Alam"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{0525DDEC-C925-45B1-9847-6B10EECC72E1}" name="Pertubuhan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{30753236-7AA4-4693-B24C-742CAA8C26E5}" name="Agama"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{FB5A0C69-03A9-4211-8A02-EDD5A66544AD}" name="Komunikasi"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{D560E911-BF63-4572-BF1B-4AF1C36BB0F6}" name="Kata Sifat"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{0B8CAF0B-9853-4166-868E-F5DFCF10FF93}" name="Filter 4"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{E41D096E-0ABB-48D0-A4ED-16352B60F84D}" name="Filter 2"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{33596B96-C2AA-4CF3-93FF-CB3D5E438131}" name="Negeri"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{4484A6DE-93A6-4A06-9698-3E212A1F4069}" name="Filter 3"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{4B29C85D-8F4B-41C5-98E1-179F34C547AD}" name="Perasaan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{E033F24B-222D-4C10-9E81-2CD13F2D27CA}" name="Pendidikan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{1C914825-B774-497B-9951-7424A275C6C8}" name="Filter 1"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{DC196AA5-A4AE-4C93-995D-C8FA5331B2E2}" name="Kecacatan"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{88CF1269-A498-4F96-8096-DF9A248D182F}" name="Keluarga"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{191CE3A5-E0F7-4A5A-A27B-B2DCD098BF72}" name="Benda"/>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{18217A88-0981-418C-ABFA-AC931682F80F}" name="Binatang"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{B7D1E82B-A5E5-4C14-9C86-B61A78ED8084}" name="Pekerjaan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{D6318188-C0E0-4364-A149-FD9E8D671A1B}" name="Buah"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{2039A978-ADAF-4711-8B07-046A7AD53BA6}" name="Pakaian"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{F436789B-C5EA-41CB-8359-78C305F1E83A}" name="Makanan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{BE442BB6-3A31-442F-B924-D13D0F598ECC}" name="Kata Penghubung"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{7B44AC12-E6B4-4313-993B-10F7132B892F}" name="Budaya"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{DBDF39FA-7899-4557-B3BC-352C416503A3}" name="Warna"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{3A76F548-2F88-4245-B104-5C766A91C956}" name="Kata Kerja"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{9DF68346-E0CA-4FA3-B5D1-1AD86B191463}" name="Kata Ganti Nama"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{560CED10-97E3-4B8F-9E2D-42501DEDD37A}" name="Haiwan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{48CE27A7-5499-4811-A41E-787093C14E7E}" name="Kata Bantu"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{AABB1EE6-8061-4BBE-83FC-087E9C58414A}" name="Kata Tanya"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{DE900718-0161-4792-8EAB-C58F78F69250}" name="Kerajaan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{9E4183D2-CC5A-4D20-BB9A-2F013C0CE815}" name="Angka"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{9E47DD61-E6DE-488B-80BA-967A50C8AB36}" name="Pengangkutan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{92BEF0B2-FF4A-4089-8EE6-8E4DADA938AF}" name="Tempat - Bangunan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{0ECEE141-0B77-44E5-A6DE-68B5A15450B4}" name="Kesihatan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{49E7F3CE-F40C-4FED-BEF8-26F090EE4EAB}" name="Badan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{C6F25ED8-01F5-4EC6-BA59-11F1B290E9F7}" name="Sukan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{1A8878F0-0412-4D55-9C2F-095CAD9E6CFA}" name="Ucapan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{43C9EAE1-EEE7-465A-B2FE-FCC5D6144576}" name="Masa"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{FAE9710F-D2BA-4EBD-88A7-23B01C8DBCFC}" name="Arah"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{AF68C2CF-34E8-443E-B4ED-BB66CB150D6B}" name="Alam"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{030204D7-095F-4354-969B-56C1AA7143AE}" name="Pertubuhan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{3D296FF4-2091-4F77-BB20-5342594B263E}" name="Agama"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{A856CC1B-B362-4556-ACE2-C976256EBF5B}" name="Komunikasi"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{8BD75489-4874-47F0-8DF3-393379AB259B}" name="Kata Sifat"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{724DC91F-FF1E-468C-B992-B1D0F51CCC52}" name="Filter 4"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{CA698D16-9134-4DB4-984A-29693DB788A8}" name="Filter 2"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{0909C5DC-ED19-4D4A-9DB0-5392CF96C4D4}" name="Negeri"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{EF393267-77E9-4937-B374-A059A55A3DDA}" name="Filter 3"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{EBA9F249-1672-448E-8531-16FD1942FCAD}" name="Perasaan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{8232B643-36E7-487B-B1D6-FD3DA06BF1E9}" name="Pendidikan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{E460850B-B72B-48C4-B246-11D0D04F03F5}" name="Filter 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{743AD89C-320C-4C4C-BC5F-7EC0A02EECDE}" name="Kecacatan"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{A7B4F8D0-C2B2-4D23-888B-901C02EDA207}" name="Keluarga"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{C330DD12-F7AD-4A16-8E93-F60E7DD26815}" name="Benda"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{D8E7AD2B-1D6A-4A53-BADF-5738E01F788C}" name="Binatang"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14781" uniqueCount="3209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14782" uniqueCount="3209">
   <si>
     <t>Perkataan</t>
   </si>
@@ -10496,6 +10496,12 @@
     <t>Toliet</t>
   </si>
   <si>
+    <t>Isyarat Baru/Isyarat Baru</t>
+  </si>
+  <si>
+    <t>New Signs/New Signs</t>
+  </si>
+  <si>
     <t>Home</t>
   </si>
   <si>
@@ -10518,19 +10524,13 @@
   </si>
   <si>
     <t>Places/Transportation</t>
-  </si>
-  <si>
-    <t>Isyarat Baru/Isyarat Baru</t>
-  </si>
-  <si>
-    <t>New Signs/New Signs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="35">
+  <fonts count="36">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -10706,6 +10706,10 @@
       <color theme="5"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -10751,7 +10755,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -11027,6 +11031,9 @@
     </xf>
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="35" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -67544,23 +67551,23 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{EB148AC7-BEAD-4132-98AC-E5E0C12786AC}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{49E7F3CE-F40C-4FED-BEF8-26F090EE4EAB}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$562:$L$572"/>
     </customSheetView>
-    <customSheetView guid="{76526F03-6BB6-47C6-A22D-8CED733D2C92}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{0ECEE141-0B77-44E5-A6DE-68B5A15450B4}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$429:$L$462">
         <sortState ref="A429:L462">
           <sortCondition ref="A429:A462"/>
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{88CF1269-A498-4F96-8096-DF9A248D182F}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{A7B4F8D0-C2B2-4D23-888B-901C02EDA207}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$533:$L$565"/>
     </customSheetView>
-    <customSheetView guid="{DC196AA5-A4AE-4C93-995D-C8FA5331B2E2}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{743AD89C-320C-4C4C-BC5F-7EC0A02EECDE}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$521:$L$531"/>
     </customSheetView>
-    <customSheetView guid="{33596B96-C2AA-4CF3-93FF-CB3D5E438131}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{0909C5DC-ED19-4D4A-9DB0-5392CF96C4D4}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$551:$L$565">
         <filterColumn colId="6">
           <filters>
@@ -67572,14 +67579,14 @@
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{4366E692-EA63-470F-AD6B-F16D89BA7A13}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{F436789B-C5EA-41CB-8359-78C305F1E83A}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$119:$L$149">
         <sortState ref="A119:L149">
           <sortCondition ref="A119:A149"/>
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{E41D096E-0ABB-48D0-A4ED-16352B60F84D}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{CA698D16-9134-4DB4-984A-29693DB788A8}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$N$1125">
         <filterColumn colId="13">
           <filters>
@@ -67588,20 +67595,20 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{D560E911-BF63-4572-BF1B-4AF1C36BB0F6}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{8BD75489-4874-47F0-8DF3-393379AB259B}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$891:$L$1023"/>
     </customSheetView>
-    <customSheetView guid="{D8E019AC-D677-4A71-A7A7-F65745991DC9}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AF68C2CF-34E8-443E-B4ED-BB66CB150D6B}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$37:$L$69"/>
     </customSheetView>
-    <customSheetView guid="{2CC30FC2-C6C4-4FBA-8A83-09C3EDAFCB1A}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{92BEF0B2-FF4A-4089-8EE6-8E4DADA938AF}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$75:$L$157">
         <sortState ref="A75:L157">
           <sortCondition ref="A75:A157"/>
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{30753236-7AA4-4693-B24C-742CAA8C26E5}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{3D296FF4-2091-4F77-BB20-5342594B263E}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$2:$L$36">
         <filterColumn colId="6">
           <filters>
@@ -67610,13 +67617,13 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{D1D0E9F4-CDA8-4E5B-93DD-F2C29EAD6080}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{1A8878F0-0412-4D55-9C2F-095CAD9E6CFA}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$970:$L$993"/>
     </customSheetView>
-    <customSheetView guid="{4900EDE6-BCBD-49E0-843B-3969248BB0EF}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AABB1EE6-8061-4BBE-83FC-087E9C58414A}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$335:$L$346"/>
     </customSheetView>
-    <customSheetView guid="{29953007-05A1-4AA5-AF83-C71F0162324C}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{43C9EAE1-EEE7-465A-B2FE-FCC5D6144576}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$718:$L$769">
         <filterColumn colId="4">
           <filters>
@@ -67629,35 +67636,35 @@
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{52071FA0-C79C-4E2C-9B82-5FC05209D4E7}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{D6318188-C0E0-4364-A149-FD9E8D671A1B}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$770:$L$793"/>
     </customSheetView>
-    <customSheetView guid="{98404195-76EE-4140-9039-AD3068CC13E6}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{DE900718-0161-4792-8EAB-C58F78F69250}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1009:$L$1031"/>
     </customSheetView>
-    <customSheetView guid="{C3F86223-1CE5-44C1-87CE-40666E8A308F}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{FAE9710F-D2BA-4EBD-88A7-23B01C8DBCFC}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$710:$L$724"/>
     </customSheetView>
-    <customSheetView guid="{0525DDEC-C925-45B1-9847-6B10EECC72E1}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{030204D7-095F-4354-969B-56C1AA7143AE}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1039:$L$1074"/>
     </customSheetView>
-    <customSheetView guid="{4B29C85D-8F4B-41C5-98E1-179F34C547AD}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{EBA9F249-1672-448E-8531-16FD1942FCAD}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$832:$L$863"/>
     </customSheetView>
-    <customSheetView guid="{E033F24B-222D-4C10-9E81-2CD13F2D27CA}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{8232B643-36E7-487B-B1D6-FD3DA06BF1E9}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$775:$L$811">
         <sortState ref="A775:L811">
           <sortCondition ref="A775:A811"/>
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{578123A8-10D5-4CF4-BC99-156B0063D202}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{3A76F548-2F88-4245-B104-5C766A91C956}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$803:$L$874"/>
     </customSheetView>
-    <customSheetView guid="{FB5A0C69-03A9-4211-8A02-EDD5A66544AD}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{A856CC1B-B362-4556-ACE2-C976256EBF5B}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$573:$L$584"/>
     </customSheetView>
-    <customSheetView guid="{05E28A09-23CF-4F91-95FB-5F959B17C232}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{B7D1E82B-A5E5-4C14-9C86-B61A78ED8084}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$728:$L$774">
         <filterColumn colId="6">
           <filters>
@@ -67669,24 +67676,24 @@
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{85A2FC98-A2B5-4E0D-AA36-AF69AE3B83B5}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{560CED10-97E3-4B8F-9E2D-42501DEDD37A}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$267:$H$314">
         <sortState ref="A267:H314">
           <sortCondition ref="A267:A314"/>
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{6FC2398D-0036-45FB-A79D-B7AEBC0EB69B}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{9E47DD61-E6DE-488B-80BA-967A50C8AB36}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$565:$L$574">
         <sortState ref="A565:L574">
           <sortCondition ref="A565:A574"/>
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{C56FDD5D-C848-4EA9-8EC0-B3E8FFB57F91}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{BE442BB6-3A31-442F-B924-D13D0F598ECC}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$875:$L$890"/>
     </customSheetView>
-    <customSheetView guid="{191CE3A5-E0F7-4A5A-A27B-B2DCD098BF72}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{C330DD12-F7AD-4A16-8E93-F60E7DD26815}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$144:$L$266">
         <filterColumn colId="11">
           <filters>
@@ -67698,10 +67705,10 @@
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{361013E5-E895-48D0-B579-FC88480C5F47}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{48CE27A7-5499-4811-A41E-787093C14E7E}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$794:$L$802"/>
     </customSheetView>
-    <customSheetView guid="{0B8CAF0B-9853-4166-868E-F5DFCF10FF93}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{724DC91F-FF1E-468C-B992-B1D0F51CCC52}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$O$1125">
         <filterColumn colId="2">
           <filters>
@@ -67719,7 +67726,7 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{4484A6DE-93A6-4A06-9698-3E212A1F4069}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{EF393267-77E9-4937-B374-A059A55A3DDA}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$O$1125">
         <filterColumn colId="13">
           <filters>
@@ -67728,36 +67735,36 @@
         </filterColumn>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{1C914825-B774-497B-9951-7424A275C6C8}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{E460850B-B72B-48C4-B246-11D0D04F03F5}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$1:$O$1125"/>
     </customSheetView>
-    <customSheetView guid="{986591FF-6F24-4023-8AC1-D53F01184713}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{9E4183D2-CC5A-4D20-BB9A-2F013C0CE815}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$77:$L$128"/>
     </customSheetView>
-    <customSheetView guid="{A984F94B-0BB4-4433-89DB-AFDFBD6AE7F9}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{7B44AC12-E6B4-4313-993B-10F7132B892F}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$315:$L$334">
         <sortState ref="A315:L334">
           <sortCondition ref="A315:A334"/>
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{440974C0-07E2-4054-AD03-D6D4230CA7A2}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{9DF68346-E0CA-4FA3-B5D1-1AD86B191463}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$573:$L$591"/>
     </customSheetView>
-    <customSheetView guid="{4CF85566-B44C-4CE0-B041-FF442715F5FB}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{2039A978-ADAF-4711-8B07-046A7AD53BA6}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$625:$L$658"/>
     </customSheetView>
-    <customSheetView guid="{941CA0B9-8F0E-40BD-8E17-11D8E91E25A7}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{C6F25ED8-01F5-4EC6-BA59-11F1B290E9F7}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$923:$L$960">
         <sortState ref="A923:L960">
           <sortCondition ref="A923:A960"/>
         </sortState>
       </autoFilter>
     </customSheetView>
-    <customSheetView guid="{DE8783DB-61C2-4EA7-A572-E71C0795FEA1}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{DBDF39FA-7899-4557-B3BC-352C416503A3}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$994:$L$1005"/>
     </customSheetView>
-    <customSheetView guid="{18217A88-0981-418C-ABFA-AC931682F80F}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{D8E7AD2B-1D6A-4A53-BADF-5738E01F788C}" filter="1" showAutoFilter="1">
       <autoFilter ref="$A$267:$L$314"/>
     </customSheetView>
   </customSheetViews>
@@ -67772,11 +67779,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
+    <dataValidation type="list" allowBlank="1" sqref="C2:C1580">
+      <formula1>Group!$A$3:$A1580</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="D2:D1580">
-      <formula1>Group!$B$2:$B1580</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C2:C1580">
-      <formula1>Group!$A$2:$A1580</formula1>
+      <formula1>Group!$B$3:$B1580</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J2:J1580">
       <formula1>"Yes,No"</formula1>
@@ -68662,426 +68669,428 @@
     </row>
     <row r="2">
       <c r="A2" s="92" t="s">
-        <v>1321</v>
+        <v>3199</v>
       </c>
       <c r="B2" s="92" t="s">
-        <v>1322</v>
-      </c>
-      <c r="C2" s="92"/>
+        <v>3200</v>
+      </c>
+      <c r="C2" s="92" t="s">
+        <v>3201</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="93" t="s">
+        <v>1321</v>
+      </c>
+      <c r="B3" s="93" t="s">
+        <v>1322</v>
+      </c>
+      <c r="C3" s="93"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="94" t="s">
         <v>1418</v>
       </c>
-      <c r="B3" s="93" t="s">
+      <c r="B4" s="94" t="s">
         <v>1419</v>
       </c>
-      <c r="C3" s="93"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="92" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="92" t="s">
-        <v>3199</v>
-      </c>
+      <c r="C4" s="94"/>
     </row>
     <row r="5">
       <c r="A5" s="93" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="93" t="s">
+        <v>3201</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="94" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="95" t="s">
+      <c r="B6" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="93" t="s">
-        <v>3199</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="92" t="s">
-        <v>167</v>
-      </c>
-      <c r="B6" s="94" t="s">
-        <v>168</v>
-      </c>
-      <c r="C6" s="92" t="s">
-        <v>3199</v>
+      <c r="C6" s="94" t="s">
+        <v>3201</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="93" t="s">
+        <v>167</v>
+      </c>
+      <c r="B7" s="95" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" s="93" t="s">
+        <v>3201</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="94" t="s">
         <v>1616</v>
       </c>
-      <c r="B7" s="93" t="s">
+      <c r="B8" s="94" t="s">
         <v>1617</v>
       </c>
-      <c r="C7" s="93"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="92" t="s">
-        <v>1769</v>
-      </c>
-      <c r="B8" s="94" t="s">
-        <v>3200</v>
-      </c>
-      <c r="C8" s="92"/>
+      <c r="C8" s="94"/>
     </row>
     <row r="9">
       <c r="A9" s="93" t="s">
+        <v>1769</v>
+      </c>
+      <c r="B9" s="95" t="s">
+        <v>3202</v>
+      </c>
+      <c r="C9" s="93"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="94" t="s">
         <v>1804</v>
       </c>
-      <c r="B9" s="93" t="s">
+      <c r="B10" s="94" t="s">
         <v>1805</v>
       </c>
-      <c r="C9" s="93"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="92" t="s">
-        <v>1901</v>
-      </c>
-      <c r="B10" s="92" t="s">
-        <v>1902</v>
-      </c>
-      <c r="C10" s="92"/>
+      <c r="C10" s="94"/>
     </row>
     <row r="11">
       <c r="A11" s="93" t="s">
+        <v>1901</v>
+      </c>
+      <c r="B11" s="93" t="s">
+        <v>1902</v>
+      </c>
+      <c r="C11" s="93"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="94" t="s">
         <v>1953</v>
       </c>
-      <c r="B11" s="93" t="s">
+      <c r="B12" s="94" t="s">
         <v>1954</v>
       </c>
-      <c r="C11" s="93"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="92" t="s">
-        <v>2060</v>
-      </c>
-      <c r="B12" s="92" t="s">
-        <v>2061</v>
-      </c>
-      <c r="C12" s="92"/>
+      <c r="C12" s="94"/>
     </row>
     <row r="13">
       <c r="A13" s="93" t="s">
+        <v>2060</v>
+      </c>
+      <c r="B13" s="93" t="s">
+        <v>2061</v>
+      </c>
+      <c r="C13" s="93"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="94" t="s">
         <v>2100</v>
       </c>
-      <c r="B13" s="93" t="s">
+      <c r="B14" s="94" t="s">
         <v>2101</v>
       </c>
-      <c r="C13" s="93"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="92" t="s">
-        <v>2172</v>
-      </c>
-      <c r="B14" s="92" t="s">
-        <v>2173</v>
-      </c>
-      <c r="C14" s="92" t="s">
-        <v>3199</v>
-      </c>
+      <c r="C14" s="94"/>
     </row>
     <row r="15">
       <c r="A15" s="93" t="s">
+        <v>2172</v>
+      </c>
+      <c r="B15" s="93" t="s">
+        <v>2173</v>
+      </c>
+      <c r="C15" s="93" t="s">
+        <v>3201</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="94" t="s">
         <v>2323</v>
       </c>
-      <c r="B15" s="93" t="s">
+      <c r="B16" s="94" t="s">
         <v>2324</v>
       </c>
-      <c r="C15" s="93" t="s">
-        <v>3199</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="92" t="s">
-        <v>2721</v>
-      </c>
-      <c r="B16" s="92" t="s">
-        <v>2722</v>
-      </c>
-      <c r="C16" s="92" t="s">
-        <v>3199</v>
+      <c r="C16" s="94" t="s">
+        <v>3201</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="93" t="s">
+        <v>2721</v>
+      </c>
+      <c r="B17" s="93" t="s">
+        <v>2722</v>
+      </c>
+      <c r="C17" s="93" t="s">
+        <v>3201</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="94" t="s">
         <v>206</v>
       </c>
-      <c r="B17" s="93" t="s">
+      <c r="B18" s="94" t="s">
         <v>207</v>
       </c>
-      <c r="C17" s="93" t="s">
-        <v>3199</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="92" t="s">
-        <v>238</v>
-      </c>
-      <c r="B18" s="92" t="s">
-        <v>239</v>
-      </c>
-      <c r="C18" s="92" t="s">
-        <v>3199</v>
+      <c r="C18" s="94" t="s">
+        <v>3201</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="93" t="s">
+        <v>238</v>
+      </c>
+      <c r="B19" s="93" t="s">
+        <v>239</v>
+      </c>
+      <c r="C19" s="93" t="s">
+        <v>3201</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="94" t="s">
         <v>308</v>
       </c>
-      <c r="B19" s="95" t="s">
+      <c r="B20" s="96" t="s">
         <v>309</v>
       </c>
-      <c r="C19" s="93" t="s">
-        <v>3199</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="92" t="s">
-        <v>2770</v>
-      </c>
-      <c r="B20" s="92" t="s">
-        <v>2771</v>
-      </c>
-      <c r="C20" s="92" t="s">
-        <v>3199</v>
+      <c r="C20" s="94" t="s">
+        <v>3201</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="93" t="s">
+        <v>2770</v>
+      </c>
+      <c r="B21" s="93" t="s">
+        <v>2771</v>
+      </c>
+      <c r="C21" s="93" t="s">
+        <v>3201</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="94" t="s">
         <v>407</v>
       </c>
-      <c r="B21" s="93" t="s">
+      <c r="B22" s="94" t="s">
         <v>408</v>
       </c>
-      <c r="C21" s="93"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="92" t="s">
-        <v>2826</v>
-      </c>
-      <c r="B22" s="92" t="s">
-        <v>2827</v>
-      </c>
-      <c r="C22" s="92"/>
+      <c r="C22" s="94"/>
     </row>
     <row r="23">
       <c r="A23" s="93" t="s">
+        <v>2826</v>
+      </c>
+      <c r="B23" s="93" t="s">
+        <v>2827</v>
+      </c>
+      <c r="C23" s="93"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="94" t="s">
         <v>2927</v>
       </c>
-      <c r="B23" s="93" t="s">
+      <c r="B24" s="94" t="s">
         <v>2928</v>
       </c>
-      <c r="C23" s="93"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="92" t="s">
-        <v>463</v>
-      </c>
-      <c r="B24" s="92" t="s">
-        <v>464</v>
-      </c>
-      <c r="C24" s="92"/>
+      <c r="C24" s="94"/>
     </row>
     <row r="25">
       <c r="A25" s="93" t="s">
+        <v>463</v>
+      </c>
+      <c r="B25" s="93" t="s">
+        <v>464</v>
+      </c>
+      <c r="C25" s="93"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="94" t="s">
         <v>587</v>
       </c>
-      <c r="B25" s="93" t="s">
+      <c r="B26" s="94" t="s">
         <v>588</v>
       </c>
-      <c r="C25" s="93"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="92" t="s">
-        <v>563</v>
-      </c>
-      <c r="B26" s="92" t="s">
-        <v>564</v>
-      </c>
-      <c r="C26" s="92"/>
+      <c r="C26" s="94"/>
     </row>
     <row r="27">
       <c r="A27" s="93" t="s">
-        <v>641</v>
+        <v>563</v>
       </c>
       <c r="B27" s="93" t="s">
-        <v>642</v>
+        <v>564</v>
       </c>
       <c r="C27" s="93"/>
     </row>
     <row r="28">
       <c r="A28" s="94" t="s">
+        <v>641</v>
+      </c>
+      <c r="B28" s="94" t="s">
+        <v>642</v>
+      </c>
+      <c r="C28" s="94"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="95" t="s">
         <v>726</v>
       </c>
-      <c r="B28" s="94" t="s">
+      <c r="B29" s="95" t="s">
         <v>727</v>
       </c>
-      <c r="C28" s="92"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="93" t="s">
+      <c r="C29" s="93"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="94" t="s">
         <v>603</v>
       </c>
-      <c r="B29" s="93" t="s">
+      <c r="B30" s="94" t="s">
         <v>604</v>
       </c>
-      <c r="C29" s="93"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="92" t="s">
-        <v>749</v>
-      </c>
-      <c r="B30" s="92" t="s">
-        <v>750</v>
-      </c>
-      <c r="C30" s="92" t="s">
-        <v>3199</v>
-      </c>
+      <c r="C30" s="94"/>
     </row>
     <row r="31">
       <c r="A31" s="93" t="s">
+        <v>749</v>
+      </c>
+      <c r="B31" s="93" t="s">
+        <v>750</v>
+      </c>
+      <c r="C31" s="93" t="s">
+        <v>3201</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="94" t="s">
         <v>814</v>
       </c>
-      <c r="B31" s="93" t="s">
+      <c r="B32" s="94" t="s">
         <v>815</v>
       </c>
-      <c r="C31" s="93" t="s">
-        <v>3199</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="92" t="s">
-        <v>2989</v>
-      </c>
-      <c r="B32" s="92" t="s">
-        <v>2990</v>
-      </c>
-      <c r="C32" s="92" t="s">
-        <v>3199</v>
+      <c r="C32" s="94" t="s">
+        <v>3201</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="93" t="s">
+        <v>2989</v>
+      </c>
+      <c r="B33" s="93" t="s">
+        <v>2990</v>
+      </c>
+      <c r="C33" s="93" t="s">
+        <v>3201</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="94" t="s">
         <v>869</v>
       </c>
-      <c r="B33" s="93" t="s">
+      <c r="B34" s="94" t="s">
         <v>870</v>
       </c>
-      <c r="C33" s="93" t="s">
-        <v>3199</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="92" t="s">
-        <v>3010</v>
-      </c>
-      <c r="B34" s="92" t="s">
-        <v>3011</v>
-      </c>
-      <c r="C34" s="92" t="s">
-        <v>3199</v>
+      <c r="C34" s="94" t="s">
+        <v>3201</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="93" t="s">
+        <v>3010</v>
+      </c>
+      <c r="B35" s="93" t="s">
+        <v>3011</v>
+      </c>
+      <c r="C35" s="93" t="s">
+        <v>3201</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="94" t="s">
         <v>981</v>
       </c>
-      <c r="B35" s="93" t="s">
+      <c r="B36" s="94" t="s">
         <v>982</v>
       </c>
-      <c r="C35" s="93" t="s">
-        <v>3199</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="92" t="s">
-        <v>1081</v>
-      </c>
-      <c r="B36" s="92" t="s">
-        <v>1082</v>
-      </c>
-      <c r="C36" s="92" t="s">
-        <v>3199</v>
+      <c r="C36" s="94" t="s">
+        <v>3201</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="93" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B37" s="93" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C37" s="93" t="s">
+        <v>3201</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="94" t="s">
         <v>3054</v>
       </c>
-      <c r="B37" s="93" t="s">
+      <c r="B38" s="94" t="s">
         <v>3055</v>
       </c>
-      <c r="C37" s="93" t="s">
-        <v>3199</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="92" t="s">
-        <v>1102</v>
-      </c>
-      <c r="B38" s="92" t="s">
-        <v>1103</v>
-      </c>
-      <c r="C38" s="92"/>
+      <c r="C38" s="94" t="s">
+        <v>3201</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="93" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B39" s="93" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C39" s="93"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="94" t="s">
         <v>3074</v>
       </c>
-      <c r="B39" s="93" t="s">
+      <c r="B40" s="94" t="s">
         <v>3075</v>
       </c>
-      <c r="C39" s="93"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="92" t="s">
-        <v>1133</v>
-      </c>
-      <c r="B40" s="92" t="s">
-        <v>1134</v>
-      </c>
-      <c r="C40" s="92"/>
+      <c r="C40" s="94"/>
     </row>
     <row r="41">
       <c r="A41" s="93" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B41" s="93" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C41" s="93"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="94" t="s">
         <v>1172</v>
       </c>
-      <c r="B41" s="93" t="s">
+      <c r="B42" s="94" t="s">
         <v>1173</v>
       </c>
-      <c r="C41" s="93"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="92" t="s">
-        <v>1244</v>
-      </c>
-      <c r="B42" s="92" t="s">
-        <v>1245</v>
-      </c>
-      <c r="C42" s="92"/>
+      <c r="C42" s="94"/>
     </row>
     <row r="43">
       <c r="A43" s="93" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B43" s="93" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C43" s="93"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="94" t="s">
         <v>3109</v>
       </c>
-      <c r="B43" s="93" t="s">
+      <c r="B44" s="94" t="s">
         <v>3110</v>
       </c>
-      <c r="C43" s="93"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="92" t="s">
-        <v>3201</v>
-      </c>
-      <c r="B44" s="92" t="s">
-        <v>3202</v>
-      </c>
-      <c r="C44" s="92"/>
+      <c r="C44" s="94"/>
     </row>
     <row r="45">
       <c r="A45" s="93" t="s">
@@ -69093,31 +69102,31 @@
       <c r="C45" s="93"/>
     </row>
     <row r="46">
-      <c r="A46" s="92" t="s">
+      <c r="A46" s="94" t="s">
         <v>3205</v>
       </c>
-      <c r="B46" s="92" t="s">
+      <c r="B46" s="94" t="s">
         <v>3206</v>
       </c>
-      <c r="C46" s="92"/>
+      <c r="C46" s="94"/>
     </row>
     <row r="47">
       <c r="A47" s="93" t="s">
+        <v>3207</v>
+      </c>
+      <c r="B47" s="93" t="s">
+        <v>3208</v>
+      </c>
+      <c r="C47" s="93"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="94" t="s">
         <v>3143</v>
       </c>
-      <c r="B47" s="93" t="s">
+      <c r="B48" s="94" t="s">
         <v>3144</v>
       </c>
-      <c r="C47" s="93"/>
-    </row>
-    <row r="48">
-      <c r="A48" s="95" t="s">
-        <v>3207</v>
-      </c>
-      <c r="B48" s="95" t="s">
-        <v>3208</v>
-      </c>
-      <c r="C48" s="95"/>
+      <c r="C48" s="94"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>